<commit_message>
working on the SIR model and estimating beta and gamma
</commit_message>
<xml_diff>
--- a/reports/motivation from numbers.xlsx
+++ b/reports/motivation from numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gjnet\code_projects\covid_forecast\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593A5A68-81C2-4123-8C17-5EACF46E65B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A348459-7D40-471C-AA99-4E22046D3E1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FF43D415-4E94-45FB-A108-ADE048EF64A6}"/>
   </bookViews>
@@ -196,8 +196,256 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Deaths</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1839</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4534</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11176</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67911</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>167400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>412641</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1017160</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2507298</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6180490</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15234908</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37554048</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>92570729</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>228186847</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>351000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A72B-4A76-955C-C1F6AF513C74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recovered</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1057</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2606</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6424</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15836</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>96223</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>237190</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>584672</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1441216</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3552598</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8757154</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21586385</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>53210440</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>131163734</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>323318604</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>796980359</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1964556584</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4842631980</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7449000000</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A72B-4A76-955C-C1F6AF513C74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$1</c:f>
@@ -318,129 +566,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Deaths</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>746</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1839</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4534</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11176</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27550</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>67911</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>167400</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>412641</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1017160</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2507298</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6180490</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>15234908</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>37554048</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>92570729</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>228186847</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>351000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A72B-4A76-955C-C1F6AF513C74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -452,147 +577,7 @@
         <c:smooth val="0"/>
         <c:axId val="1626853279"/>
         <c:axId val="1217484127"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="2"/>
-                <c:order val="2"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Recovered</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$B$31</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0</c:formatCode>
-                      <c:ptCount val="30"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>71</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>174</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>429</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1057</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>2606</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>6424</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>15836</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>39036</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>96223</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>237190</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>584672</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>1441216</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>3552598</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>8757154</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>21586385</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>53210440</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>131163734</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>323318604</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>796980359</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>1964556584</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>4842631980</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>7449000000</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-A72B-4A76-955C-C1F6AF513C74}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1626853279"/>
@@ -633,7 +618,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1668,7 +1653,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>